<commit_message>
included changes based on the discussions during the presentation
</commit_message>
<xml_diff>
--- a/data/data_driven_cv_data.xlsx
+++ b/data/data_driven_cv_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lares/Documents/carpentries/data_driven_cv-main/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405C18E4-722A-DB43-B885-E0191DA18C9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4C1C6C-554E-9046-8BC0-075E1C88434E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7620" yWindow="580" windowWidth="28040" windowHeight="14900" activeTab="10" xr2:uid="{F39B64C4-0EAB-E54C-9DAD-28AA668AE6DA}"/>
+    <workbookView xWindow="4520" yWindow="580" windowWidth="25760" windowHeight="14900" activeTab="4" xr2:uid="{F39B64C4-0EAB-E54C-9DAD-28AA668AE6DA}"/>
   </bookViews>
   <sheets>
     <sheet name="admin_services" sheetId="3" r:id="rId1"/>
@@ -209,7 +209,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="69">
   <si>
     <t>title</t>
   </si>
@@ -407,6 +407,15 @@
   </si>
   <si>
     <t>include_in_resume</t>
+  </si>
+  <si>
+    <t>Carpentries Instructors Development Meeting</t>
+  </si>
+  <si>
+    <t>December</t>
+  </si>
+  <si>
+    <t>Data-driven CV</t>
   </si>
 </sst>
 </file>
@@ -962,7 +971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90399CE6-1B85-E746-B0A9-367BE265EE22}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -1291,8 +1300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B56E59DD-B714-EB43-9DD1-8B39EF184637}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1376,7 +1385,7 @@
         <v>30</v>
       </c>
       <c r="D3">
-        <v>2022</v>
+        <v>2016</v>
       </c>
       <c r="E3" t="s">
         <v>31</v>
@@ -1434,7 +1443,7 @@
         <v>30</v>
       </c>
       <c r="D5">
-        <v>2021</v>
+        <v>2017</v>
       </c>
       <c r="E5" t="s">
         <v>30</v>
@@ -1449,7 +1458,7 @@
         <v>36</v>
       </c>
       <c r="I5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -1463,7 +1472,7 @@
         <v>30</v>
       </c>
       <c r="D6">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E6" t="s">
         <v>30</v>
@@ -1507,7 +1516,7 @@
         <v>38</v>
       </c>
       <c r="I7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -1729,10 +1738,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BA1C487-1357-FD47-BC8E-81AB45E0B8A1}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H24"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1796,6 +1805,32 @@
         <v>50</v>
       </c>
       <c r="H2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3">
+        <v>2022</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
skeleton data for the repo
</commit_message>
<xml_diff>
--- a/data/data_driven_cv_data.xlsx
+++ b/data/data_driven_cv_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lares/Documents/carpentries/data_driven_cv-main/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4C1C6C-554E-9046-8BC0-075E1C88434E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973C346A-001B-944E-A9E8-C2F878812855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4520" yWindow="580" windowWidth="25760" windowHeight="14900" activeTab="4" xr2:uid="{F39B64C4-0EAB-E54C-9DAD-28AA668AE6DA}"/>
+    <workbookView xWindow="24180" yWindow="5340" windowWidth="34000" windowHeight="22600" activeTab="10" xr2:uid="{F39B64C4-0EAB-E54C-9DAD-28AA668AE6DA}"/>
   </bookViews>
   <sheets>
     <sheet name="admin_services" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
     <definedName name="education" localSheetId="3">education!$A$1:$F$6</definedName>
     <definedName name="experience" localSheetId="4">experience!$A$1:$H$37</definedName>
     <definedName name="grants_and_awards" localSheetId="5">grants_and_awards!$A$1:$H$6</definedName>
-    <definedName name="invited_teaching" localSheetId="6">invited_teaching!$A$1:$H$8</definedName>
+    <definedName name="invited_teaching" localSheetId="6">invited_teaching!$A$1:$H$11</definedName>
     <definedName name="presentations" localSheetId="7">presentations!$A$1:$H$24</definedName>
     <definedName name="proyects" localSheetId="8">projects!$A$1:$H$5</definedName>
     <definedName name="publications" localSheetId="9">publications!$A$1:$I$5</definedName>
@@ -209,7 +209,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="51">
   <si>
     <t>title</t>
   </si>
@@ -271,7 +271,7 @@
     <t>UW-Madison Department of Spanish and Portuguese</t>
   </si>
   <si>
-    <t>Fall</t>
+    <t xml:space="preserve">Spring </t>
   </si>
   <si>
     <t xml:space="preserve">Member of the Linguistic Society of America </t>
@@ -310,36 +310,6 @@
     <t xml:space="preserve">Lead the migration of the data science platform to servers on premise which includes meeting and negotiating with the vendor representatives, collaborating with the Linux Team to properly set up VM configurations, and managing the data science applications themselves. </t>
   </si>
   <si>
-    <t>Collaborate with researchers to adopt data science and computational strategies to improve their workflows.</t>
-  </si>
-  <si>
-    <t>Team up with other units on campus in order to pool resources and reduce pain points for researchers using these computational resources.</t>
-  </si>
-  <si>
-    <t>Graduate Project Assistant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Engineered a solution for the Limnology Department by modifying their R workflows to access their data through a PostGres database. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assisted several researchers with issues regarding data wrangling, shiny apps publication, and data storage and management. </t>
-  </si>
-  <si>
-    <t>Participated in campus-wide events to promote data science tools.</t>
-  </si>
-  <si>
-    <t>Analyzed 8 years of longitudinal data in order to produce qualitative and quantitative insights leading to improvements in the Electronic Lab Notebook service.</t>
-  </si>
-  <si>
-    <t>Produced hundreds of visualizations to better convey findings and trends contained in the data.</t>
-  </si>
-  <si>
-    <t>Spring</t>
-  </si>
-  <si>
-    <t>June</t>
-  </si>
-  <si>
     <t xml:space="preserve">August </t>
   </si>
   <si>
@@ -349,16 +319,7 @@
     <t xml:space="preserve">UW-Madison Faculty Council of The Department of Spanish and Portuguese </t>
   </si>
   <si>
-    <t xml:space="preserve">Data Wrangling </t>
-  </si>
-  <si>
-    <t>The Carpentries</t>
-  </si>
-  <si>
-    <t>Keep your Class Presentations Updated Painlessly with Rmarkdown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IT Professionals Conference </t>
+    <t xml:space="preserve">UW-Madison Libraries </t>
   </si>
   <si>
     <t>UW-Madison, WI</t>
@@ -373,7 +334,7 @@
     <t>Collaborate with Dr. Rajiv Rao to analyze and visualize the data produced by a longitudinal project which monitored voice onset time (VOT) development of students living in a domestic language immersion program.</t>
   </si>
   <si>
-    <t>Carry out the quantitative analysis of the data gathered by this project. The results will be published in a peer-reviewed journal.</t>
+    <t xml:space="preserve">December </t>
   </si>
   <si>
     <t>area</t>
@@ -388,34 +349,19 @@
     <t>Spanish, English, Italian, Portuguese, Japanese, Yucatec Mayan</t>
   </si>
   <si>
-    <t xml:space="preserve">Computer Languages </t>
-  </si>
-  <si>
-    <t>R,  LaTeX, Python, HTML, CSS, Bash, SQL, Markdown, YAML, GIT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Additional Technical Skills </t>
-  </si>
-  <si>
-    <t>Jupyter Labs + Notebooks, AWS, Canvas LMS, BlackBoard LMS, Praat, Microsoft Office</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Additional Soft Skills </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aikidoist 3rd degree black belt, dog trainer, ceramicist </t>
-  </si>
-  <si>
     <t>include_in_resume</t>
   </si>
   <si>
-    <t>Carpentries Instructors Development Meeting</t>
-  </si>
-  <si>
-    <t>December</t>
-  </si>
-  <si>
-    <t>Data-driven CV</t>
+    <t>Madison WI</t>
+  </si>
+  <si>
+    <t>Instructors Development Meetings from the Carpentries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep your resume updated with a data-driven CV </t>
+  </si>
+  <si>
+    <t>R Basics</t>
   </si>
 </sst>
 </file>
@@ -969,10 +915,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90399CE6-1B85-E746-B0A9-367BE265EE22}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -989,10 +935,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1015,10 +961,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -1036,84 +982,6 @@
         <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1232,7 +1100,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:G6"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1265,7 +1133,7 @@
         <v>8</v>
       </c>
       <c r="G1" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1298,10 +1166,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B56E59DD-B714-EB43-9DD1-8B39EF184637}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1342,7 +1210,7 @@
         <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1371,209 +1239,6 @@
         <v>32</v>
       </c>
       <c r="I2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3">
-        <v>2016</v>
-      </c>
-      <c r="E3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4">
-        <v>2022</v>
-      </c>
-      <c r="E4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5">
-        <v>2017</v>
-      </c>
-      <c r="E5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5">
-        <v>2022</v>
-      </c>
-      <c r="G5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" t="s">
-        <v>36</v>
-      </c>
-      <c r="I5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6">
-        <v>2020</v>
-      </c>
-      <c r="E6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6">
-        <v>2022</v>
-      </c>
-      <c r="G6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" t="s">
-        <v>37</v>
-      </c>
-      <c r="I6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7">
-        <v>2021</v>
-      </c>
-      <c r="E7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7">
-        <v>2022</v>
-      </c>
-      <c r="G7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8">
-        <v>2021</v>
-      </c>
-      <c r="E8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8">
-        <v>2022</v>
-      </c>
-      <c r="G8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" t="s">
-        <v>39</v>
-      </c>
-      <c r="I8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9">
-        <v>2021</v>
-      </c>
-      <c r="E9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9">
-        <v>2022</v>
-      </c>
-      <c r="G9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" t="s">
-        <v>40</v>
-      </c>
-      <c r="I9" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1630,10 +1295,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -1664,7 +1329,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H8"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1707,25 +1372,25 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
       </c>
       <c r="D2">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2">
-        <v>2022</v>
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="H2" t="s">
         <v>11</v>
@@ -1738,10 +1403,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BA1C487-1357-FD47-BC8E-81AB45E0B8A1}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1784,16 +1449,16 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
         <v>48</v>
       </c>
-      <c r="B2" t="s">
-        <v>49</v>
-      </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D2">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
@@ -1802,35 +1467,9 @@
         <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3">
-        <v>2022</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1841,10 +1480,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{680B7B8E-970D-5047-A082-1C89D3C869A8}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:H5"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1860,7 +1499,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1886,13 +1525,13 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D2">
         <v>2021</v>
@@ -1907,33 +1546,7 @@
         <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3">
-        <v>2021</v>
-      </c>
-      <c r="E3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>